<commit_message>
Updates: Updated the DataManager file references wherever I could find, also the relative paths Updated the code and ran the "test_login" test case Updated the code and ran the "test_login_ddt-1" test case - For this one, code replaced Updated the code and ran for "Dashboard Selection" -  For this one, code replaced
</commit_message>
<xml_diff>
--- a/TestData/DataManager.xlsx
+++ b/TestData/DataManager.xlsx
@@ -5,24 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Pycharm\3DX_pythonProject\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\test-automation\feature\Code_merge\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C02D9-F365-4A29-A91A-88A303CF07B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D2A52A-B42B-496C-BA10-86DEFAD7DD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Inputs" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="document" sheetId="3" r:id="rId3"/>
+    <sheet name="transmittal" sheetId="5" r:id="rId4"/>
+    <sheet name="Placeholder" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="158">
   <si>
     <t>username</t>
   </si>
@@ -283,6 +285,221 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>DocType</t>
+  </si>
+  <si>
+    <t>Serial No</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>WO</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>How Many</t>
+  </si>
+  <si>
+    <t>folder_path (for revise PH)</t>
+  </si>
+  <si>
+    <t>ASB - As-Built Drawing</t>
+  </si>
+  <si>
+    <t>PH sequence6</t>
+  </si>
+  <si>
+    <t>Region02</t>
+  </si>
+  <si>
+    <t>Organization9</t>
+  </si>
+  <si>
+    <t>AVC - Audio Visual</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>03 - Design</t>
+  </si>
+  <si>
+    <t>Original file path</t>
+  </si>
+  <si>
+    <t>D:\My Projects\Selenium\Original_upload\02-0000100082-AAE-LTR-000001_XX.pdf</t>
+  </si>
+  <si>
+    <t>MDL - BIM Model</t>
+  </si>
+  <si>
+    <t>PH_created</t>
+  </si>
+  <si>
+    <t>DAT - Data Sheet</t>
+  </si>
+  <si>
+    <t>DRG - Drawing</t>
+  </si>
+  <si>
+    <t>Document  for TRA</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Filters selection</t>
+  </si>
+  <si>
+    <t>TraType</t>
+  </si>
+  <si>
+    <t>TRAReason</t>
+  </si>
+  <si>
+    <t>TRA_Response</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Asset code</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Work Order</t>
+  </si>
+  <si>
+    <t>Design related</t>
+  </si>
+  <si>
+    <t>Info Requested</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>sraut</t>
+  </si>
+  <si>
+    <t>02-DAH-LAN-3DM-345004</t>
+  </si>
+  <si>
+    <t>Auto-created Title 1</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>IMP_ReasonForIssue</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Test Excel subject 1</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>0000100113</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>02A</t>
+  </si>
+  <si>
+    <t>Auto Info 1</t>
+  </si>
+  <si>
+    <t>Auto Message 1</t>
+  </si>
+  <si>
+    <t>tra_created</t>
+  </si>
+  <si>
+    <t>GC-TRA-000053</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ARC - Architectural</t>
+  </si>
+  <si>
+    <t>psuraneni</t>
+  </si>
+  <si>
+    <t>Test@2022</t>
+  </si>
+  <si>
+    <t>OwnedByMe</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Reason For Issue</t>
+  </si>
+  <si>
+    <t>Response Required</t>
+  </si>
+  <si>
+    <t>Transmittal Category</t>
+  </si>
+  <si>
+    <t>Work Order/Service Order</t>
+  </si>
+  <si>
+    <t>02-DAH-LAN-3DM-245004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+															Request For Information
+														</t>
+  </si>
+  <si>
+    <t>IFD - Issued for Design</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Auto-Created TRA 1</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>0000000000 - IMP Wide</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Test Message created</t>
   </si>
 </sst>
 </file>
@@ -314,7 +531,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,8 +568,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -388,12 +617,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -444,6 +706,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -727,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,14 +1422,462 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="G3" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G5" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G6" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G7" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G8" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G9" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G10" s="29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G11" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D6D914-98E5-44BB-A609-6E43D31E8456}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="P3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04649D4-B85F-4770-9E36-CF59CEEA629B}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2">
+        <v>110023</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>